<commit_message>
on the way to fix imageupdate
</commit_message>
<xml_diff>
--- a/ILP/NN/Book1.xlsx
+++ b/ILP/NN/Book1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1759921\Documents\code\matlab\Neural-Networks\ILP\NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7875B50F-6AD5-455F-A5A6-6CF02D038970}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D64BD8-A3EA-4CFF-A085-841C4E4E6961}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>flow5</t>
   </si>
@@ -109,13 +110,19 @@
   </si>
   <si>
     <t>56.95s</t>
+  </si>
+  <si>
+    <t>RGR</t>
+  </si>
+  <si>
+    <t>Romdom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,8 +144,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,8 +172,23 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -159,13 +196,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,10 +279,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="5" builtinId="10"/>
+    <cellStyle name="Output" xfId="4" builtinId="21"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -510,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -606,7 +703,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
@@ -624,211 +721,1276 @@
         <v>24.39</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.2</v>
+      </c>
+    </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1">
-        <v>23.41</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1">
+        <v>23.41</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="5">
-        <v>45.69</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0.57699999999999996</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="9">
-        <v>82.86</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5">
-        <v>34.22</v>
+        <v>45.69</v>
       </c>
       <c r="D11" s="7">
-        <v>0.34300000000000003</v>
+        <v>0.57699999999999996</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="9">
+        <v>82.86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="5">
+        <v>34.22</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="9">
         <v>73.16</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="1">
-        <v>41.16</v>
-      </c>
-      <c r="D14" s="6">
-        <v>1</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1</v>
-      </c>
-      <c r="F14" s="5">
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1">
-        <v>70.72</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.56669999999999998</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1">
-        <v>39.700000000000003</v>
+        <v>41.16</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="1">
-        <v>44.51</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.4</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1">
-        <v>4.91</v>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1">
+        <v>70.72</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.56669999999999998</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1">
+        <v>39.700000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44.51</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1">
+        <v>4.91</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="1">
-        <v>75.239999999999995</v>
-      </c>
-      <c r="D20" s="3">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D20" s="7">
+        <v>6.6699999999999995E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="1">
-        <v>105.85</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.375</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1">
-        <v>31.07</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1">
+        <v>75.239999999999995</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1">
+        <v>105.85</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1">
+        <v>31.07</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{943922B4-3D52-464F-A1AC-6B981F67487E}">
+  <dimension ref="A1:AG10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AG20" sqref="AG20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A1" s="10">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10">
+        <v>0.40000571874086699</v>
+      </c>
+      <c r="C1" s="10">
+        <v>0.18487765262754099</v>
+      </c>
+      <c r="D1" s="10">
+        <v>0.41511662863159199</v>
+      </c>
+      <c r="E1" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1" s="10">
+        <v>0</v>
+      </c>
+      <c r="G1" s="10">
+        <v>0</v>
+      </c>
+      <c r="H1" s="11">
+        <v>0.13571428571428601</v>
+      </c>
+      <c r="I1" s="11">
+        <v>0.13571428571428601</v>
+      </c>
+      <c r="J1" s="11">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="K1" s="11">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="L1" s="11">
+        <v>0.23749999999999999</v>
+      </c>
+      <c r="M1" s="11">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="N1" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="O1" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="P1" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="Q1" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="R1" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="S1" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="T1" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="U1" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="V1" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="W1" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="X1" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="Y1" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="Z1" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="AA1" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AB1" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="AC1" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AD1" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AE1" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AF1" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="AG1" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A2" s="10">
+        <v>2.67634190239904E-2</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0.93213611554213505</v>
+      </c>
+      <c r="C2" s="10">
+        <v>4.11004654338743E-2</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10">
+        <v>0</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11">
+        <v>6.4285714285714293E-2</v>
+      </c>
+      <c r="I2" s="11">
+        <v>6.4285714285714293E-2</v>
+      </c>
+      <c r="J2" s="11">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="K2" s="11">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="L2" s="11">
+        <v>0.1125</v>
+      </c>
+      <c r="M2" s="11">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="N2" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="O2" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="P2" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="Q2" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="R2" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="S2" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="T2" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="U2" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="V2" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="W2" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="X2" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="Y2" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="Z2" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="AA2" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AB2" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="AC2" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AD2" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AE2" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AF2" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="AG2" s="12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A3" s="10">
+        <v>0</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0.42095972572016499</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.144779299259997</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.43426097501983801</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0.121428571428571</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0.121428571428571</v>
+      </c>
+      <c r="J3" s="11">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="K3" s="11">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="L3" s="11">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="M3" s="11">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="N3" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="O3" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="P3" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="R3" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="S3" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="T3" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="U3" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="V3" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="W3" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="X3" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="Y3" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="Z3" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="AA3" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AB3" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="AC3" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AD3" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AE3" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AF3" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="AG3" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A4" s="10">
+        <v>0.401369379659896</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.165107244831184</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.43352337550892001</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0.13571428571428601</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.13571428571428601</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="L4" s="11">
+        <v>0.23749999999999999</v>
+      </c>
+      <c r="M4" s="11">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="N4" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="O4" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="P4" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="R4" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="S4" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="T4" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="U4" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="V4" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="W4" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="X4" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="Y4" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="Z4" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="AA4" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AB4" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="AC4" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AD4" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AE4" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AF4" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="AG4" s="12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A5" s="10">
+        <v>0</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0.40701934692976199</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.18307557861599399</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.40990507445424401</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0.121428571428571</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0.121428571428571</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="M5" s="11">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="N5" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="O5" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="P5" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="R5" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="S5" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="T5" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="U5" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="V5" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="W5" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="X5" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="Y5" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="Z5" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="AA5" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AB5" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="AC5" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AD5" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AE5" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AF5" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="AG5" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A6" s="10">
+        <v>0</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.415671208907962</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.149712660308572</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0.434616130783466</v>
+      </c>
+      <c r="H6" s="11">
+        <v>7.8571428571428598E-2</v>
+      </c>
+      <c r="I6" s="11">
+        <v>7.8571428571428598E-2</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="K6" s="11">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0.13750000000000001</v>
+      </c>
+      <c r="M6" s="11">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="N6" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="O6" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="P6" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="R6" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="S6" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="T6" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="U6" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="V6" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="W6" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="X6" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="Y6" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="Z6" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="AA6" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AB6" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="AC6" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AD6" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AE6" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AF6" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="AG6" s="12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
+        <v>0</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.80850442113697796</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.19149557886302199</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0.121428571428571</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.121428571428571</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="K7" s="11">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="M7" s="11">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="N7" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="O7" s="12">
+        <v>0.1875</v>
+      </c>
+      <c r="P7" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="R7" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="S7" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="T7" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="U7" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="V7" s="12">
+        <v>0.1875</v>
+      </c>
+      <c r="W7" s="12">
+        <v>0.1875</v>
+      </c>
+      <c r="X7" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="Y7" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="Z7" s="12">
+        <v>0.1875</v>
+      </c>
+      <c r="AA7" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="AB7" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AC7" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="AD7" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="AE7" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="AF7" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AG7" s="12">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
+        <v>0.91096717469135302</v>
+      </c>
+      <c r="B8" s="10">
+        <v>8.9032825308647201E-2</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>6.4285714285714293E-2</v>
+      </c>
+      <c r="I8" s="11">
+        <v>6.4285714285714293E-2</v>
+      </c>
+      <c r="J8" s="11">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="K8" s="11">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0.1125</v>
+      </c>
+      <c r="M8" s="11">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="N8" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="O8" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="P8" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="R8" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="S8" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="T8" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="U8" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="V8" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="W8" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="X8" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="Y8" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="Z8" s="12">
+        <v>6.25E-2</v>
+      </c>
+      <c r="AA8" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AB8" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="AC8" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AD8" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AE8" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AF8" s="12">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="AG8" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A9" s="10">
+        <v>0.90378994228645504</v>
+      </c>
+      <c r="B9" s="10">
+        <v>9.6210057713545197E-2</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <v>9.2857142857142902E-2</v>
+      </c>
+      <c r="I9" s="11">
+        <v>9.2857142857142902E-2</v>
+      </c>
+      <c r="J9" s="11">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="M9" s="11">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="N9" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="O9" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="P9" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="R9" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="S9" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="T9" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="U9" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="V9" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="W9" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="X9" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="Y9" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="Z9" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="AA9" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AB9" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="AC9" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AD9" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AE9" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="AF9" s="12">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="AG9" s="12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A10" s="10">
+        <v>0</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.41577578155030298</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.14989917206561801</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.43432504638407898</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0.13571428571428601</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0.13571428571428601</v>
+      </c>
+      <c r="J10" s="11">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0.23749999999999999</v>
+      </c>
+      <c r="M10" s="11">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="N10" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="O10" s="12">
+        <v>0.1875</v>
+      </c>
+      <c r="P10" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="Q10" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="R10" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="S10" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="T10" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="U10" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="V10" s="12">
+        <v>0.1875</v>
+      </c>
+      <c r="W10" s="12">
+        <v>0.1875</v>
+      </c>
+      <c r="X10" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="Y10" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="Z10" s="12">
+        <v>0.1875</v>
+      </c>
+      <c r="AA10" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="AB10" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AC10" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="AD10" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="AE10" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="AF10" s="12">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="AG10" s="12">
+        <v>0.15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
first 40 test data for flow20
</commit_message>
<xml_diff>
--- a/ILP/NN/Book1.xlsx
+++ b/ILP/NN/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1759921\Documents\code\matlab\Neural-Networks\ILP\NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235C8EF2-9AFE-4CE8-84B9-721FEF9101BB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD09BA4-9BF1-45CC-BD64-27159A54E782}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,15 +90,9 @@
     <t>33.02s</t>
   </si>
   <si>
-    <t>1.71h</t>
-  </si>
-  <si>
     <t>0.05s</t>
   </si>
   <si>
-    <t>44.88s</t>
-  </si>
-  <si>
     <t>2.7h</t>
   </si>
   <si>
@@ -124,6 +118,12 @@
   </si>
   <si>
     <t>1.44s</t>
+  </si>
+  <si>
+    <t>48.48s</t>
+  </si>
+  <si>
+    <t>1.58h</t>
   </si>
 </sst>
 </file>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,7 +621,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
@@ -681,17 +681,17 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5">
-        <v>23.74</v>
+        <v>24.33</v>
       </c>
       <c r="D10" s="7">
         <v>0.76800000000000002</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5">
-        <v>3.355</v>
+        <v>21.73</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -699,10 +699,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="5">
-        <v>45.69</v>
+        <v>48.4</v>
       </c>
       <c r="D11" s="7">
         <v>0.57699999999999996</v>
@@ -714,20 +714,20 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="5">
-        <v>34.22</v>
+        <v>35.89</v>
       </c>
       <c r="D12" s="7">
         <v>0.34300000000000003</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="9">
-        <v>73.16</v>
+        <v>85.43</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -752,10 +752,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1">
-        <v>41.16</v>
+        <v>39.04</v>
       </c>
       <c r="D16" s="6">
         <v>1</v>
@@ -772,17 +772,17 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1">
-        <v>45.88</v>
+        <v>49.09</v>
       </c>
       <c r="D17" s="3">
-        <v>0.5</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1">
-        <v>12.27</v>
+        <v>54.91</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -790,35 +790,35 @@
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1">
-        <v>70.72</v>
+        <v>1193.3</v>
       </c>
       <c r="D18" s="2">
-        <v>0.56669999999999998</v>
+        <v>0.51929999999999998</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1">
-        <v>39.700000000000003</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C19" s="1">
-        <v>44.51</v>
+        <v>675.07</v>
       </c>
       <c r="D19" s="3">
-        <v>0.4</v>
+        <v>0.25269999999999998</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1">
-        <v>4.91</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -839,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C23" s="1">
         <v>75.239999999999995</v>
@@ -859,7 +859,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1">
         <v>72.44</v>
@@ -875,7 +875,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25" s="1">
         <v>105.85</v>
@@ -890,10 +890,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C26" s="1">
         <v>71.78</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D27" s="7">
         <v>0.05</v>

</xml_diff>

<commit_message>
fix the bug in umgUpdate, which may produce an undefined value previously
</commit_message>
<xml_diff>
--- a/ILP/NN/Book1.xlsx
+++ b/ILP/NN/Book1.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1759921\Documents\code\matlab\Neural-Networks\ILP\NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD09BA4-9BF1-45CC-BD64-27159A54E782}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C2173C-A172-48DB-8A6C-06698A644382}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sgdm" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -93,15 +93,9 @@
     <t>0.05s</t>
   </si>
   <si>
-    <t>2.7h</t>
-  </si>
-  <si>
     <t>0.08s</t>
   </si>
   <si>
-    <t>56.95s</t>
-  </si>
-  <si>
     <t>RGR</t>
   </si>
   <si>
@@ -117,13 +111,19 @@
     <t>0.75s</t>
   </si>
   <si>
-    <t>1.44s</t>
-  </si>
-  <si>
     <t>48.48s</t>
   </si>
   <si>
     <t>1.58h</t>
+  </si>
+  <si>
+    <t>2.4h</t>
+  </si>
+  <si>
+    <t>2.1s</t>
+  </si>
+  <si>
+    <t>94.16s</t>
   </si>
 </sst>
 </file>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,7 +621,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
@@ -681,7 +681,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5">
         <v>24.33</v>
@@ -699,7 +699,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="5">
         <v>48.4</v>
@@ -714,7 +714,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1">
         <v>39.04</v>
@@ -772,7 +772,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1">
         <v>49.09</v>
@@ -805,10 +805,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1">
         <v>675.07</v>
@@ -839,10 +839,10 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1">
-        <v>75.239999999999995</v>
+        <v>64.91</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
@@ -859,54 +859,64 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C24" s="1">
-        <v>72.44</v>
+        <v>124.66</v>
       </c>
       <c r="D24" s="2">
-        <v>0.4375</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+        <v>0.51849999999999996</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.84850000000000003</v>
+      </c>
+      <c r="F24" s="1">
+        <v>136.6</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="1">
-        <v>105.85</v>
+        <v>269.45999999999998</v>
       </c>
       <c r="D25" s="2">
-        <v>0.375</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>0.44350000000000001</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.8075</v>
+      </c>
       <c r="F25" s="1">
-        <v>31.07</v>
+        <v>646.1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C26" s="1">
-        <v>71.78</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+        <v>156.36000000000001</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.21049999999999999</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="F26" s="1">
+        <v>635.79999999999995</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D27" s="7">
         <v>0.05</v>
@@ -914,5 +924,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
compare different assignment methods result
</commit_message>
<xml_diff>
--- a/ILP/NN/Book1.xlsx
+++ b/ILP/NN/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1759921\Documents\code\matlab\Neural-Networks\ILP\NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C2173C-A172-48DB-8A6C-06698A644382}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA181D2-4E89-4ED4-BC82-A5EE80CBCB30}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>flow5</t>
   </si>
@@ -72,27 +72,9 @@
     <t>flow20</t>
   </si>
   <si>
-    <t>0.11s</t>
-  </si>
-  <si>
-    <t>0.46s</t>
-  </si>
-  <si>
     <t>0.01s</t>
   </si>
   <si>
-    <t>20.44s</t>
-  </si>
-  <si>
-    <t>100.00s</t>
-  </si>
-  <si>
-    <t>33.02s</t>
-  </si>
-  <si>
-    <t>0.05s</t>
-  </si>
-  <si>
     <t>0.08s</t>
   </si>
   <si>
@@ -102,18 +84,9 @@
     <t>Romdom</t>
   </si>
   <si>
-    <t>0.37s</t>
-  </si>
-  <si>
     <t>0.03s</t>
   </si>
   <si>
-    <t>0.75s</t>
-  </si>
-  <si>
-    <t>48.48s</t>
-  </si>
-  <si>
     <t>1.58h</t>
   </si>
   <si>
@@ -124,13 +97,64 @@
   </si>
   <si>
     <t>94.16s</t>
+  </si>
+  <si>
+    <t>1.07s</t>
+  </si>
+  <si>
+    <t>0.04s</t>
+  </si>
+  <si>
+    <t>49.73s</t>
+  </si>
+  <si>
+    <t>80.96s</t>
+  </si>
+  <si>
+    <t>0.51s</t>
+  </si>
+  <si>
+    <t>32.75s</t>
+  </si>
+  <si>
+    <t>0.49s</t>
+  </si>
+  <si>
+    <t>0.15s</t>
+  </si>
+  <si>
+    <t>20.69s</t>
+  </si>
+  <si>
+    <t>≈6μs</t>
+  </si>
+  <si>
+    <t>≈10μs</t>
+  </si>
+  <si>
+    <t>≈40μs</t>
+  </si>
+  <si>
+    <t>0.19s</t>
+  </si>
+  <si>
+    <t>0.56s</t>
+  </si>
+  <si>
+    <t>1.24s</t>
+  </si>
+  <si>
+    <t>2.24s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,25 +169,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -175,20 +187,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -203,15 +211,21 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -525,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -539,7 +553,7 @@
     <col min="6" max="6" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,52 +573,67 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1">
-        <v>10.82</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
+        <v>10.83</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>13</v>
+      <c r="B3" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C3" s="1">
-        <v>10.85</v>
+        <v>10.84</v>
       </c>
       <c r="D3" s="2">
-        <v>0.91539999999999999</v>
-      </c>
-      <c r="E3" s="3">
+        <v>0.92820000000000003</v>
+      </c>
+      <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="1">
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.4</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="4">
+        <v>10.84</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0.92879999999999996</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>17.95</v>
@@ -612,59 +641,74 @@
       <c r="D4" s="2">
         <v>0.63539999999999996</v>
       </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="8">
-        <v>67.180000000000007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E4" s="2">
+        <v>0.99760000000000004</v>
+      </c>
+      <c r="F4" s="4">
+        <v>67.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1">
-        <v>16.77</v>
+        <v>16.739999999999998</v>
       </c>
       <c r="D5" s="2">
-        <v>0.31459999999999999</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-      <c r="F5" s="8">
-        <v>24.39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.31819999999999998</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="7">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1">
+        <v>17.16</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.17280000000000001</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.99739999999999995</v>
+      </c>
+      <c r="F6" s="8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>17</v>
+      <c r="B9" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C9" s="1">
-        <v>23.41</v>
+        <v>23.31</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
@@ -672,87 +716,122 @@
       <c r="E9" s="6">
         <v>1</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="5">
-        <v>24.33</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0.76800000000000002</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5">
-        <v>21.73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4">
+        <v>25.07</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.81530000000000002</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.99250000000000005</v>
+      </c>
+      <c r="F10" s="4">
+        <v>89.1</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="4">
+        <v>25.11</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.81040000000000001</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.99250000000000005</v>
+      </c>
+      <c r="L10" s="4">
+        <v>89.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="5">
-        <v>48.4</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0.57699999999999996</v>
-      </c>
-      <c r="E11" s="6"/>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="4">
+        <v>58.28</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.57120000000000004</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.95169999999999999</v>
+      </c>
       <c r="F11" s="9">
-        <v>82.86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="5">
-        <v>35.89</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0.34300000000000003</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="9">
-        <v>85.43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="4">
+        <v>38.090000000000003</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.29070000000000001</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.97929999999999995</v>
+      </c>
+      <c r="F12" s="4">
+        <v>151.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="4">
+        <v>186.24</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.1678</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.96089999999999998</v>
+      </c>
+      <c r="F13" s="10">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1">
         <v>39.04</v>
@@ -763,103 +842,142 @@
       <c r="E16" s="6">
         <v>1</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1">
-        <v>49.09</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.63800000000000001</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>55.59</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.94799999999999995</v>
+      </c>
       <c r="F17" s="1">
-        <v>54.91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>106.6</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="4">
+        <v>55.56</v>
+      </c>
+      <c r="J17" s="6">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="K17" s="6">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="L17" s="4">
+        <v>134.13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1">
-        <v>1193.3</v>
+        <v>124.75</v>
       </c>
       <c r="D18" s="2">
         <v>0.51929999999999998</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="2">
+        <v>0.89</v>
+      </c>
       <c r="F18" s="1">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>463.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1">
-        <v>675.07</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0.25269999999999998</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>98.72</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="F19" s="8">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="7">
-        <v>6.6699999999999995E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="11">
+        <v>510.9</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.154</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.85729999999999995</v>
+      </c>
+      <c r="F20" s="10">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C23" s="1">
         <v>64.91</v>
       </c>
-      <c r="D23" s="3">
-        <v>1</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
         <v>1</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C24" s="1">
         <v>124.66</v>
@@ -873,13 +991,28 @@
       <c r="F24" s="1">
         <v>136.6</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="4">
+        <v>124.03</v>
+      </c>
+      <c r="J24" s="6">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="K24" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="L24" s="4">
+        <v>140.62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C25" s="1">
         <v>269.45999999999998</v>
@@ -894,12 +1027,12 @@
         <v>646.1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="C26" s="1">
         <v>156.36000000000001</v>
@@ -914,12 +1047,24 @@
         <v>635.79999999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="7">
-        <v>0.05</v>
+        <v>16</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2807.8</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.16750000000000001</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.72650000000000003</v>
+      </c>
+      <c r="F27" s="10">
+        <v>30000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
On the way to Luxembourg!
</commit_message>
<xml_diff>
--- a/ILP/NN/Book1.xlsx
+++ b/ILP/NN/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1759921\Documents\code\matlab\Neural-Networks\ILP\NN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4CB4E1-663B-49AD-9BBB-A28BEEB918E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F0FDCD-5E91-4DF5-9B34-CFB1FE51CDE8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -602,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1139,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C59FD7-C23E-4E65-A0A4-B2B3A05C9B74}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1152,7 +1152,7 @@
     <col min="5" max="5" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="12">
         <v>200</v>
       </c>
@@ -1191,8 +1191,13 @@
       <c r="F2" s="4">
         <v>66.400000000000006</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <v>400</v>
       </c>
@@ -1211,8 +1216,10 @@
       <c r="F3" s="4">
         <v>37.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="J3" s="7"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>600</v>
       </c>
@@ -1232,7 +1239,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>800</v>
       </c>
@@ -1252,7 +1259,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>1000</v>
       </c>
@@ -1272,7 +1279,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>1200</v>
       </c>
@@ -1292,7 +1299,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>1400</v>
       </c>
@@ -1312,7 +1319,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>1600</v>
       </c>
@@ -1332,7 +1339,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>1800</v>
       </c>
@@ -1352,7 +1359,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>2000</v>
       </c>
@@ -1372,12 +1379,12 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>200</v>
       </c>
@@ -1397,7 +1404,7 @@
         <v>126.9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>400</v>
       </c>
@@ -1417,7 +1424,7 @@
         <v>120.2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>600</v>
       </c>
@@ -1437,7 +1444,7 @@
         <v>120.2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>800</v>
       </c>
@@ -1593,9 +1600,9 @@
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="12">

</xml_diff>